<commit_message>
add projeto django para parte web
</commit_message>
<xml_diff>
--- a/data/base_chuva_01641010.xlsx
+++ b/data/base_chuva_01641010.xlsx
@@ -1159,7 +1159,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1226,13 +1226,13 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1600,7 +1600,7 @@
     <col min="46" max="46" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="4" t="s">
         <v>46</v>
       </c>
@@ -1876,7 +1876,7 @@
       </c>
       <c r="AT2" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="4" t="s">
         <v>48</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="4" t="s">
         <v>50</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="4" t="s">
         <v>52</v>
       </c>
@@ -2288,7 +2288,7 @@
       </c>
       <c r="AT5" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="4" t="s">
         <v>54</v>
       </c>
@@ -2426,7 +2426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="4" t="s">
         <v>56</v>
       </c>
@@ -2562,7 +2562,7 @@
       </c>
       <c r="AT7" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="4" t="s">
         <v>58</v>
       </c>
@@ -2700,7 +2700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="4" t="s">
         <v>60</v>
       </c>
@@ -2832,7 +2832,7 @@
       <c r="AS9" s="7"/>
       <c r="AT9" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="4" t="s">
         <v>62</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="4" t="s">
         <v>64</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="4" t="s">
         <v>66</v>
       </c>
@@ -3244,7 +3244,7 @@
       </c>
       <c r="AT12" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="4" t="s">
         <v>68</v>
       </c>
@@ -3382,7 +3382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="4" t="s">
         <v>70</v>
       </c>
@@ -3518,7 +3518,7 @@
       </c>
       <c r="AT14" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="4" t="s">
         <v>72</v>
       </c>
@@ -3656,7 +3656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="4" t="s">
         <v>74</v>
       </c>
@@ -3794,7 +3794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="4" t="s">
         <v>76</v>
       </c>
@@ -3930,7 +3930,7 @@
       </c>
       <c r="AT17" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="4" t="s">
         <v>78</v>
       </c>
@@ -4068,7 +4068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="4" t="s">
         <v>80</v>
       </c>
@@ -4204,7 +4204,7 @@
       </c>
       <c r="AT19" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="4" t="s">
         <v>82</v>
       </c>
@@ -4342,7 +4342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="4" t="s">
         <v>84</v>
       </c>
@@ -4474,7 +4474,7 @@
       <c r="AS21" s="7"/>
       <c r="AT21" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="4" t="s">
         <v>86</v>
       </c>
@@ -4612,7 +4612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="4" t="s">
         <v>88</v>
       </c>
@@ -4750,7 +4750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="4" t="s">
         <v>90</v>
       </c>
@@ -4886,7 +4886,7 @@
       </c>
       <c r="AT24" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="4" t="s">
         <v>92</v>
       </c>
@@ -5024,7 +5024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="4" t="s">
         <v>94</v>
       </c>
@@ -5160,7 +5160,7 @@
       </c>
       <c r="AT26" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="4" t="s">
         <v>96</v>
       </c>
@@ -5298,7 +5298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="4" t="s">
         <v>98</v>
       </c>
@@ -5436,7 +5436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="4" t="s">
         <v>100</v>
       </c>
@@ -5572,7 +5572,7 @@
       </c>
       <c r="AT29" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="4" t="s">
         <v>102</v>
       </c>
@@ -5710,7 +5710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="4" t="s">
         <v>104</v>
       </c>
@@ -5846,7 +5846,7 @@
       </c>
       <c r="AT31" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="4" t="s">
         <v>106</v>
       </c>
@@ -5984,7 +5984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="4" t="s">
         <v>108</v>
       </c>
@@ -6116,7 +6116,7 @@
       <c r="AS33" s="7"/>
       <c r="AT33" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="4" t="s">
         <v>110</v>
       </c>
@@ -6254,7 +6254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="4" t="s">
         <v>112</v>
       </c>

</xml_diff>